<commit_message>
Import two sheets from spreadsheet
</commit_message>
<xml_diff>
--- a/SimSigExport.xlsx
+++ b/SimSigExport.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukie\source\repos\SimsigImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686507AA-1BC0-404B-A324-C92B41D08F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD989990-81F3-4A55-AB6A-E26E49A44B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
   </bookViews>
   <sheets>
     <sheet name="Seed Groups" sheetId="1" r:id="rId1"/>
-    <sheet name="Timetable" sheetId="3" r:id="rId2"/>
-    <sheet name="Train Types" sheetId="2" r:id="rId3"/>
+    <sheet name="Timetable Up" sheetId="3" r:id="rId2"/>
+    <sheet name="Timetable Down" sheetId="4" r:id="rId3"/>
+    <sheet name="Train Types" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -301,9 +302,6 @@
     <t>MNMRGRN</t>
   </si>
   <si>
-    <t>Coesely</t>
-  </si>
-  <si>
     <t>COSELEY</t>
   </si>
   <si>
@@ -325,18 +323,12 @@
     <t>SNDWDUD</t>
   </si>
   <si>
-    <t>0002</t>
-  </si>
-  <si>
     <t>Galton Jn</t>
   </si>
   <si>
     <t>#GALTONJ</t>
   </si>
   <si>
-    <t>WN194(50)</t>
-  </si>
-  <si>
     <t>Seeds</t>
   </si>
   <si>
@@ -364,18 +356,6 @@
     <t>Power</t>
   </si>
   <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Bristol TM</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
     <t>1S19</t>
   </si>
   <si>
@@ -467,6 +447,18 @@
   </si>
   <si>
     <t>CL50 + Mk2s + BG</t>
+  </si>
+  <si>
+    <t>2359</t>
+  </si>
+  <si>
+    <t>0019</t>
+  </si>
+  <si>
+    <t>0034</t>
+  </si>
+  <si>
+    <t>0020</t>
   </si>
 </sst>
 </file>
@@ -563,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -577,6 +569,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -943,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52C7610-3C21-45C1-A819-83D8DB5DD38A}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,10 +950,10 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -969,7 +965,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -978,20 +974,20 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1004,20 +1000,20 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1026,15 +1022,15 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="11" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1046,7 +1042,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1055,7 +1051,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>47</v>
@@ -1077,7 +1073,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>51</v>
@@ -1110,7 +1106,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>58</v>
@@ -1161,7 +1157,7 @@
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E20" s="7"/>
     </row>
@@ -1174,7 +1170,7 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E21" s="4"/>
     </row>
@@ -1202,10 +1198,10 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1217,10 +1213,10 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1236,7 +1232,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>81</v>
@@ -1258,10 +1254,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1269,10 +1265,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1280,41 +1276,41 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1391,12 +1387,8 @@
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
@@ -1406,372 +1398,208 @@
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>107</v>
-      </c>
+      <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="D48" s="4"/>
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
-      <c r="D49" t="s">
-        <v>139</v>
-      </c>
-      <c r="E49" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>102</v>
-      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>98</v>
-      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="11" t="s">
-        <v>96</v>
-      </c>
+      <c r="D53" s="11"/>
       <c r="E53" s="11"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="11"/>
-      <c r="E54" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>92</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="11"/>
-      <c r="E56" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>84</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="D62" s="4">
-        <v>1</v>
-      </c>
-      <c r="E62" s="4">
-        <v>1</v>
-      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="4"/>
-      <c r="D63" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="D65" s="5"/>
       <c r="E65" s="5"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>66</v>
-      </c>
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="A70" s="8"/>
+      <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>52</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>50</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>48</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="D75" s="4"/>
       <c r="E75" s="4"/>
     </row>
   </sheetData>
@@ -1781,6 +1609,1134 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F9D0A2-ADCA-4890-BA88-64C3FB71B5B9}">
+  <dimension ref="A1:AD76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+    </row>
+    <row r="11" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+    </row>
+    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+    </row>
+    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+    </row>
+    <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+    </row>
+    <row r="15" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+    </row>
+    <row r="16" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="13"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="13"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H32:J53">
+    <sortCondition descending="1" ref="H32:H53"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC83C6B9-C911-4BD1-AE44-69CB7FDC537F}">
   <dimension ref="A1:X27"/>
   <sheetViews>
@@ -1883,7 +2839,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C3">
         <v>75</v>
@@ -1920,7 +2876,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C4">
         <v>75</v>
@@ -1961,7 +2917,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C5">
         <v>75</v>
@@ -2002,7 +2958,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C6">
         <v>75</v>
@@ -2041,7 +2997,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C7">
         <v>110</v>
@@ -2078,7 +3034,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C8">
         <v>110</v>
@@ -2115,7 +3071,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -2154,7 +3110,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C10">
         <v>100</v>

</xml_diff>

<commit_message>
Finish export of a weeks worth of timetables
</commit_message>
<xml_diff>
--- a/SimSigExport.xlsx
+++ b/SimSigExport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukie\source\repos\SimsigImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD989990-81F3-4A55-AB6A-E26E49A44B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519383BD-2BDB-4818-88E2-A6D61626ABE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
   </bookViews>
@@ -449,9 +449,6 @@
     <t>CL50 + Mk2s + BG</t>
   </si>
   <si>
-    <t>2359</t>
-  </si>
-  <si>
     <t>0019</t>
   </si>
   <si>
@@ -459,6 +456,9 @@
   </si>
   <si>
     <t>0020</t>
+  </si>
+  <si>
+    <t>S91</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1613,7 @@
   <dimension ref="A1:AD76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,7 +1718,9 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="E10" s="14"/>
       <c r="F10" s="13"/>
       <c r="M10" s="13"/>
@@ -1807,9 +1809,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
-        <v>134</v>
-      </c>
+      <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
         <v>76</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>68</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
         <v>55</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" s="14"/>
     </row>
@@ -2121,7 +2121,7 @@
         <v>46</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F32" s="14"/>
     </row>

</xml_diff>

<commit_message>
Updated for latest release 1.3
</commit_message>
<xml_diff>
--- a/SimSigExport.xlsx
+++ b/SimSigExport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukie\source\repos\SimsigImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA97934-BBDE-4982-A105-EB1ACA5126A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0BD7A4-BB47-43B1-A27A-69E3D546CE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
+    <workbookView xWindow="19090" yWindow="-10830" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
   </bookViews>
   <sheets>
     <sheet name="Seed Groups" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="143">
   <si>
     <t>ID</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>(2) is pathing allowance in minutes</t>
+  </si>
+  <si>
+    <t>AsRequired</t>
   </si>
 </sst>
 </file>
@@ -949,10 +952,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52C7610-3C21-45C1-A819-83D8DB5DD38A}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,16 +1058,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1072,32 +1075,26 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>121</v>
+      <c r="A14" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1105,259 +1102,267 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>57</v>
+      <c r="A16" t="s">
+        <v>121</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>61</v>
+      <c r="A18" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="A19" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
-        <v>3</v>
-      </c>
-      <c r="E23" s="4">
-        <v>3</v>
-      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>116</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B28" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>89</v>
+      <c r="A31" t="s">
+        <v>85</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>111</v>
-      </c>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>91</v>
+      <c r="A32" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="4"/>
+      <c r="A33" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="11" t="s">
-        <v>139</v>
+      <c r="E33" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>109</v>
+      <c r="A34" t="s">
+        <v>91</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
-        <v>108</v>
+      <c r="E34" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -1371,32 +1376,32 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
@@ -1444,8 +1449,8 @@
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
@@ -1458,50 +1463,51 @@
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="11"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="11"/>
-      <c r="E56" s="4"/>
+      <c r="E56" s="11"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="11"/>
@@ -1515,58 +1521,57 @@
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="E60" s="4"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
@@ -1576,23 +1581,25 @@
       <c r="E67" s="5"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
@@ -1601,26 +1608,26 @@
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="8"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
+      <c r="A74" s="8"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
@@ -1635,8 +1642,20 @@
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1646,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F9D0A2-ADCA-4890-BA88-64C3FB71B5B9}">
-  <dimension ref="A1:AD77"/>
+  <dimension ref="A1:AD79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,113 +1770,86 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-    </row>
-    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="14"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
-    </row>
-    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
     </row>
     <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="14"/>
+      <c r="A14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>76</v>
-      </c>
+      <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -1880,10 +1872,10 @@
     </row>
     <row r="15" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1910,14 +1902,16 @@
     </row>
     <row r="16" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="F16" s="14"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
@@ -1940,10 +1934,10 @@
     </row>
     <row r="17" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1968,114 +1962,150 @@
       <c r="AC17" s="14"/>
       <c r="AD17" s="14"/>
     </row>
-    <row r="18" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+    </row>
+    <row r="19" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+    </row>
+    <row r="20" spans="1:30" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="21" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>134</v>
-      </c>
+    <row r="23" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="D24" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+    <row r="25" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="26" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -2084,147 +2114,143 @@
     </row>
     <row r="27" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>58</v>
-      </c>
+    <row r="28" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>136</v>
-      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="14"/>
     </row>
-    <row r="30" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="14"/>
+    <row r="30" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="31" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="D31" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="15"/>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C33" s="14"/>
-      <c r="D33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>135</v>
-      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+    <row r="34" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
-      <c r="F34" s="13"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="13"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="13"/>
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
@@ -2235,7 +2261,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="14"/>
+      <c r="I39" s="13"/>
       <c r="J39" s="14"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -2249,7 +2275,7 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="14"/>
+      <c r="I40" s="13"/>
       <c r="J40" s="14"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
@@ -2314,8 +2340,8 @@
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
@@ -2333,7 +2359,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
+      <c r="I46" s="14"/>
       <c r="J46" s="14"/>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
@@ -2342,12 +2368,12 @@
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
+      <c r="D47" s="15"/>
       <c r="E47" s="15"/>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
+      <c r="I47" s="14"/>
       <c r="J47" s="14"/>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
@@ -2356,8 +2382,8 @@
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
@@ -2371,7 +2397,7 @@
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="E49" s="15"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
@@ -2384,12 +2410,12 @@
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="14"/>
+      <c r="I50" s="13"/>
       <c r="J50" s="14"/>
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
@@ -2398,8 +2424,8 @@
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
@@ -2412,12 +2438,12 @@
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
+      <c r="I52" s="14"/>
       <c r="J52" s="14"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
@@ -2427,7 +2453,7 @@
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
       <c r="D53" s="15"/>
-      <c r="E53" s="14"/>
+      <c r="E53" s="15"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
@@ -2445,7 +2471,7 @@
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
-      <c r="I54" s="14"/>
+      <c r="I54" s="13"/>
       <c r="J54" s="14"/>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
@@ -2460,12 +2486,12 @@
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
+      <c r="J55" s="14"/>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
       <c r="D56" s="15"/>
@@ -2473,8 +2499,8 @@
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
     </row>
@@ -2483,7 +2509,7 @@
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
       <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
+      <c r="E57" s="14"/>
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
@@ -2493,7 +2519,7 @@
       <c r="L57" s="13"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
       <c r="D58" s="15"/>
@@ -2507,11 +2533,11 @@
       <c r="L58" s="13"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+      <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
@@ -2521,11 +2547,11 @@
       <c r="L59" s="13"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
@@ -2535,7 +2561,7 @@
       <c r="L60" s="13"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -2549,11 +2575,11 @@
       <c r="L61" s="13"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="13"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
@@ -2566,8 +2592,8 @@
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
@@ -2633,7 +2659,7 @@
       <c r="L67" s="13"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+      <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="16"/>
@@ -2647,7 +2673,7 @@
       <c r="L68" s="13"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
       <c r="D69" s="16"/>
@@ -2689,7 +2715,7 @@
       <c r="L71" s="13"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
+      <c r="A72" s="13"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
       <c r="D72" s="16"/>
@@ -2717,11 +2743,11 @@
       <c r="L73" s="13"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
+      <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
@@ -2734,8 +2760,8 @@
       <c r="A75" s="13"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
@@ -2748,8 +2774,8 @@
       <c r="A76" s="13"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
@@ -2760,8 +2786,8 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
@@ -2772,9 +2798,37 @@
       <c r="K77" s="13"/>
       <c r="L77" s="13"/>
     </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H33:J54">
-    <sortCondition descending="1" ref="H33:H54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H35:J56">
+    <sortCondition descending="1" ref="H35:H56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>